<commit_message>
Added two new API tests and renamed objects
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue - Chapter 13.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue - Chapter 13.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8648E6-89C1-4E11-A51F-71391EF84AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A54FEE0-960E-40CA-82FD-EBFC87654E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="285" windowWidth="24510" windowHeight="15990" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="44">
   <si>
     <t>Feature</t>
   </si>
@@ -145,6 +145,27 @@
   </si>
   <si>
     <t>Send POST request for lookup value JSON object</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Modify lookup value with empty description</t>
+  </si>
+  <si>
+    <t>Create lookup value with empty description</t>
+  </si>
+  <si>
+    <t>Lookup value JSON object with empty description</t>
+  </si>
+  <si>
+    <t>Updated lookup value JSON object with empty description</t>
+  </si>
+  <si>
+    <t>Non-updated lookup value in database</t>
+  </si>
+  <si>
+    <t>No new lookup value in database</t>
   </si>
 </sst>
 </file>
@@ -326,6 +347,54 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -388,54 +457,6 @@
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -450,28 +471,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M22" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A1:M22" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M33" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A1:M33" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
     <tableColumn id="11" xr3:uid="{8F685D88-2001-49B6-A560-44AC61A85751}" name="Document"/>
-    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{470B84A4-8789-448A-A9D4-722FDC7901C1}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="9">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="8">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="1">
+    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="7">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -774,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,7 +1332,7 @@
         <v>Then 'Updated lookup value in database' }</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>11</v>
       </c>
@@ -1320,9 +1341,11 @@
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+      <c r="E18" s="19" t="s">
+        <v>37</v>
+      </c>
       <c r="F18" s="20" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="21"/>
@@ -1331,15 +1354,15 @@
       </c>
       <c r="J18" s="23" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0203] Create lookup value</v>
+        <v>[SCENARIO #0203] Modify lookup value with empty description</v>
       </c>
       <c r="K18" s="24" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0203] Create lookup value</v>
+        <v>//[SCENARIO #0203] Modify lookup value with empty description</v>
       </c>
       <c r="L18" s="28" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0203 'Create lookup value' {</v>
+        <v>Scenario 0203 'Modify lookup value with empty description' {</v>
       </c>
       <c r="M18" s="21"/>
     </row>
@@ -1350,26 +1373,29 @@
       <c r="B19" t="s">
         <v>18</v>
       </c>
+      <c r="E19" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="G19" t="s">
         <v>12</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I19" s="13">
         <v>203</v>
       </c>
       <c r="J19" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Lookup value JSON object</v>
+        <v>[GIVEN] Committed lookup value</v>
       </c>
       <c r="K19" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Lookup value JSON object</v>
+        <v>//[GIVEN] Committed lookup value</v>
       </c>
       <c r="L19" s="26" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Lookup value JSON object'</v>
+        <v>Given 'Committed lookup value'</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1379,26 +1405,29 @@
       <c r="B20" t="s">
         <v>18</v>
       </c>
+      <c r="E20" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="G20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="I20" s="13">
         <v>203</v>
       </c>
       <c r="J20" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Send POST request for lookup value JSON object</v>
+        <v>[GIVEN] Updated lookup value JSON object with empty description</v>
       </c>
       <c r="K20" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Send POST request for lookup value JSON object</v>
+        <v>//[GIVEN] Updated lookup value JSON object with empty description</v>
       </c>
       <c r="L20" s="26" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Send POST request for lookup value JSON object'</v>
+        <v>Given 'Updated lookup value JSON object with empty description'</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1408,26 +1437,29 @@
       <c r="B21" t="s">
         <v>18</v>
       </c>
+      <c r="E21" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="I21" s="13">
         <v>203</v>
       </c>
       <c r="J21" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] New lookup value in response</v>
+        <v>[WHEN] Send PATCH request for lookup value JSON object</v>
       </c>
       <c r="K21" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] New lookup value in response</v>
+        <v>//[WHEN] Send PATCH request for lookup value JSON object</v>
       </c>
       <c r="L21" s="26" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'New lookup value in response'</v>
+        <v>When 'Send PATCH request for lookup value JSON object'</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1437,52 +1469,397 @@
       <c r="B22" t="s">
         <v>18</v>
       </c>
+      <c r="E22" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="G22" t="s">
         <v>14</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I22" s="13">
         <v>203</v>
       </c>
       <c r="J22" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Empty response</v>
+      </c>
+      <c r="K22" s="15" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Empty response</v>
+      </c>
+      <c r="L22" s="26" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Empty response'</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="13">
+        <v>203</v>
+      </c>
+      <c r="J23" s="14" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Non-updated lookup value in database</v>
+      </c>
+      <c r="K23" s="15" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Non-updated lookup value in database</v>
+      </c>
+      <c r="L23" s="26" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Non-updated lookup value in database' }</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="18"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="22">
+        <v>204</v>
+      </c>
+      <c r="J24" s="23" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0204] Create lookup value</v>
+      </c>
+      <c r="K24" s="24" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0204] Create lookup value</v>
+      </c>
+      <c r="L24" s="28" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0204 'Create lookup value' {</v>
+      </c>
+      <c r="M24" s="21"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="13">
+        <v>204</v>
+      </c>
+      <c r="J25" s="14" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Lookup value JSON object</v>
+      </c>
+      <c r="K25" s="15" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Lookup value JSON object</v>
+      </c>
+      <c r="L25" s="26" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value JSON object'</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I26" s="13">
+        <v>204</v>
+      </c>
+      <c r="J26" s="14" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Send POST request for lookup value JSON object</v>
+      </c>
+      <c r="K26" s="15" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Send POST request for lookup value JSON object</v>
+      </c>
+      <c r="L26" s="26" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Send POST request for lookup value JSON object'</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" s="13">
+        <v>204</v>
+      </c>
+      <c r="J27" s="14" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] New lookup value in response</v>
+      </c>
+      <c r="K27" s="15" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] New lookup value in response</v>
+      </c>
+      <c r="L27" s="26" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'New lookup value in response'</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="13">
+        <v>204</v>
+      </c>
+      <c r="J28" s="14" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[THEN] New lookup value in database</v>
       </c>
-      <c r="K22" s="15" t="str">
+      <c r="K28" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] New lookup value in database</v>
       </c>
-      <c r="L22" s="26" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'New lookup value in database' } }</v>
+      <c r="L28" s="26" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'New lookup value in database' }</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" s="18"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="22">
+        <v>205</v>
+      </c>
+      <c r="J29" s="23" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0205] Create lookup value with empty description</v>
+      </c>
+      <c r="K29" s="24" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0205] Create lookup value with empty description</v>
+      </c>
+      <c r="L29" s="28" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0205 'Create lookup value with empty description' {</v>
+      </c>
+      <c r="M29" s="21"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I30" s="13">
+        <v>205</v>
+      </c>
+      <c r="J30" s="14" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Lookup value JSON object with empty description</v>
+      </c>
+      <c r="K30" s="15" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Lookup value JSON object with empty description</v>
+      </c>
+      <c r="L30" s="26" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Lookup value JSON object with empty description'</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I31" s="13">
+        <v>205</v>
+      </c>
+      <c r="J31" s="14" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Send POST request for lookup value JSON object</v>
+      </c>
+      <c r="K31" s="15" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Send POST request for lookup value JSON object</v>
+      </c>
+      <c r="L31" s="26" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Send POST request for lookup value JSON object'</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="13">
+        <v>205</v>
+      </c>
+      <c r="J32" s="14" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Empty response</v>
+      </c>
+      <c r="K32" s="15" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Empty response</v>
+      </c>
+      <c r="L32" s="26" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Empty response'</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" s="13">
+        <v>205</v>
+      </c>
+      <c r="J33" s="14" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] No new lookup value in database</v>
+      </c>
+      <c r="K33" s="15" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] No new lookup value in database</v>
+      </c>
+      <c r="L33" s="26" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'No new lookup value in database' } }</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="15" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="51" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsBlanks" dxfId="14" priority="50">
+    <cfRule type="containsBlanks" dxfId="4" priority="50">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="13" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="16" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="17" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="18" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Third version of API tests
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue - Chapter 13.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue - Chapter 13.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A54FEE0-960E-40CA-82FD-EBFC87654E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426BCD1A-B2D5-471C-B754-33E7F9B86A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="45">
   <si>
     <t>Feature</t>
   </si>
@@ -141,12 +141,6 @@
     <t>Send DELETE request for lookup value</t>
   </si>
   <si>
-    <t>Send PATCH request for lookup value JSON object</t>
-  </si>
-  <si>
-    <t>Send POST request for lookup value JSON object</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -166,6 +160,15 @@
   </si>
   <si>
     <t>No new lookup value in database</t>
+  </si>
+  <si>
+    <t>Send PATCH request for lookup value</t>
+  </si>
+  <si>
+    <t>Send POST request for lookup value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send POST request for lookup value </t>
   </si>
 </sst>
 </file>
@@ -347,54 +350,6 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -457,6 +412,54 @@
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -471,28 +474,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M33" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M33" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:M33" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
     <tableColumn id="11" xr3:uid="{8F685D88-2001-49B6-A560-44AC61A85751}" name="Document"/>
-    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{470B84A4-8789-448A-A9D4-722FDC7901C1}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="9">
+    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="3">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="8">
+    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="7">
+    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="1">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -798,7 +801,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,22 +1259,22 @@
         <v>13</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="I15" s="13">
         <v>202</v>
       </c>
       <c r="J15" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Send PATCH request for lookup value JSON object</v>
+        <v>[WHEN] Send PATCH request for lookup value</v>
       </c>
       <c r="K15" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Send PATCH request for lookup value JSON object</v>
+        <v>//[WHEN] Send PATCH request for lookup value</v>
       </c>
       <c r="L15" s="26" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Send PATCH request for lookup value JSON object'</v>
+        <v>When 'Send PATCH request for lookup value'</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1342,10 +1345,10 @@
       <c r="C18" s="18"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="21"/>
@@ -1374,7 +1377,7 @@
         <v>18</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G19" t="s">
         <v>12</v>
@@ -1406,13 +1409,13 @@
         <v>18</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G20" t="s">
         <v>12</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I20" s="13">
         <v>203</v>
@@ -1438,28 +1441,28 @@
         <v>18</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G21" t="s">
         <v>13</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="I21" s="13">
         <v>203</v>
       </c>
       <c r="J21" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Send PATCH request for lookup value JSON object</v>
+        <v>[WHEN] Send PATCH request for lookup value</v>
       </c>
       <c r="K21" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Send PATCH request for lookup value JSON object</v>
+        <v>//[WHEN] Send PATCH request for lookup value</v>
       </c>
       <c r="L21" s="26" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Send PATCH request for lookup value JSON object'</v>
+        <v>When 'Send PATCH request for lookup value'</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1470,7 +1473,7 @@
         <v>18</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G22" t="s">
         <v>14</v>
@@ -1502,13 +1505,13 @@
         <v>18</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G23" t="s">
         <v>14</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I23" s="13">
         <v>203</v>
@@ -1587,7 +1590,7 @@
         <v>Given 'Lookup value JSON object'</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -1598,22 +1601,22 @@
         <v>13</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="I26" s="13">
         <v>204</v>
       </c>
       <c r="J26" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Send POST request for lookup value JSON object</v>
+        <v xml:space="preserve">[WHEN] Send POST request for lookup value </v>
       </c>
       <c r="K26" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Send POST request for lookup value JSON object</v>
+        <v xml:space="preserve">//[WHEN] Send POST request for lookup value </v>
       </c>
       <c r="L26" s="26" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Send POST request for lookup value JSON object'</v>
+        <v>When 'Send POST request for lookup value '</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1684,10 +1687,10 @@
       <c r="C29" s="18"/>
       <c r="D29" s="19"/>
       <c r="E29" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="20" t="s">
         <v>37</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>39</v>
       </c>
       <c r="G29" s="18"/>
       <c r="H29" s="21"/>
@@ -1716,13 +1719,13 @@
         <v>18</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G30" t="s">
         <v>12</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I30" s="13">
         <v>205</v>
@@ -1748,28 +1751,28 @@
         <v>18</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G31" t="s">
         <v>13</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="I31" s="13">
         <v>205</v>
       </c>
       <c r="J31" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Send POST request for lookup value JSON object</v>
+        <v>[WHEN] Send POST request for lookup value</v>
       </c>
       <c r="K31" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Send POST request for lookup value JSON object</v>
+        <v>//[WHEN] Send POST request for lookup value</v>
       </c>
       <c r="L31" s="26" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Send POST request for lookup value JSON object'</v>
+        <v>When 'Send POST request for lookup value'</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -1780,7 +1783,7 @@
         <v>18</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G32" t="s">
         <v>14</v>
@@ -1812,13 +1815,13 @@
         <v>18</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G33" t="s">
         <v>14</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I33" s="13">
         <v>205</v>
@@ -1838,28 +1841,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="5" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="51" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsBlanks" dxfId="4" priority="50">
+    <cfRule type="containsBlanks" dxfId="14" priority="50">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="3" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="2" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>